<commit_message>
fix iqc nom ep 1E17
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/OT_IQC.xlsx
+++ b/lib/PHPExcel/templates/OT_IQC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,6 +22,40 @@
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Pierrick Gonnet</author>
+  </authors>
+  <commentList>
+    <comment ref="N5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="22"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GPM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="22"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Write equipment(s) number here</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -179,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -249,6 +283,19 @@
       <sz val="10"/>
       <color rgb="FF255663"/>
       <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="22"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="22"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1359,7 +1406,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1403,6 +1449,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1959,7 +2006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1981,7 +2028,7 @@
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" customWidth="1"/>
     <col min="17" max="17" width="7.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="109" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="108" customWidth="1"/>
     <col min="19" max="19" width="17.28515625" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" customWidth="1"/>
@@ -1991,7 +2038,7 @@
       <c r="P1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="104"/>
+      <c r="R1" s="103"/>
       <c r="S1" s="36" t="s">
         <v>0</v>
       </c>
@@ -2014,19 +2061,19 @@
       <c r="N2" s="26"/>
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
-      <c r="R2" s="105"/>
+      <c r="R2" s="104"/>
       <c r="S2" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R3" s="106"/>
+      <c r="R3" s="105"/>
       <c r="S3" s="38" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R4" s="107"/>
+      <c r="R4" s="106"/>
       <c r="S4" s="40" t="s">
         <v>4</v>
       </c>
@@ -2051,7 +2098,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="31"/>
-      <c r="R5" s="105"/>
+      <c r="R5" s="104"/>
       <c r="S5" s="37" t="s">
         <v>7</v>
       </c>
@@ -2075,7 +2122,7 @@
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="27"/>
-      <c r="R6" s="108"/>
+      <c r="R6" s="107"/>
       <c r="S6" s="39" t="s">
         <v>10</v>
       </c>
@@ -2099,13 +2146,13 @@
       <c r="N7" s="41"/>
       <c r="O7" s="41"/>
       <c r="P7" s="42"/>
-      <c r="R7" s="104"/>
+      <c r="R7" s="103"/>
       <c r="S7" s="36" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R8" s="105"/>
+      <c r="R8" s="104"/>
       <c r="S8" s="37" t="s">
         <v>14</v>
       </c>
@@ -2132,35 +2179,35 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="R9" s="106"/>
+      <c r="R9" s="105"/>
       <c r="S9" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="123"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="125"/>
-      <c r="N10" s="126"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="127"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="125"/>
+      <c r="O10" s="123"/>
+      <c r="P10" s="126"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="127" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="128"/>
+      <c r="A12" s="127"/>
       <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
@@ -2180,7 +2227,7 @@
       <c r="P12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="128"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
@@ -2226,12 +2273,12 @@
       <c r="P13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R13" s="109" t="s">
+      <c r="R13" s="108" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="128"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="67"/>
       <c r="C14" s="68"/>
       <c r="D14" s="68" t="str">
@@ -2263,11 +2310,11 @@
         <v/>
       </c>
       <c r="B15" s="73" t="str">
-        <f>IF(OldData!B15="","",OldData!B15)</f>
-        <v/>
-      </c>
-      <c r="C15" s="103" t="str">
-        <f>IF(OldData!C15="","",OldData!C15)</f>
+        <f>IF(OldData!B15="","",MID(OldData!B15,2,9999))</f>
+        <v/>
+      </c>
+      <c r="C15" s="128" t="str">
+        <f>IF(OldData!C15="","",MID(OldData!C15,2,9999))</f>
         <v/>
       </c>
       <c r="D15" s="32" t="str">
@@ -2323,7 +2370,7 @@
         <v/>
       </c>
       <c r="Q15" s="81"/>
-      <c r="R15" s="110" t="str">
+      <c r="R15" s="109" t="str">
         <f t="shared" ref="R15:R46" si="0">B15&amp;C15</f>
         <v/>
       </c>
@@ -2334,11 +2381,11 @@
         <v/>
       </c>
       <c r="B16" s="53" t="str">
-        <f>IF(OldData!B16="","",OldData!B16)</f>
+        <f>IF(OldData!B16="","",MID(OldData!B16,2,9999))</f>
         <v/>
       </c>
       <c r="C16" s="54" t="str">
-        <f>IF(OldData!C16="","",OldData!C16)</f>
+        <f>IF(OldData!C16="","",MID(OldData!C16,2,9999))</f>
         <v/>
       </c>
       <c r="D16" s="32" t="str">
@@ -2393,7 +2440,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R16,'New Data'!$R$16:$R$115,0),CELL("colonne",P16)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R16,'New Data'!$R$16:$R$115,0),CELL("colonne",P16)-3)),IF(OldData!P16="","",OldData!P16))</f>
         <v/>
       </c>
-      <c r="R16" s="110" t="str">
+      <c r="R16" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2404,11 +2451,11 @@
         <v/>
       </c>
       <c r="B17" s="53" t="str">
-        <f>IF(OldData!B17="","",OldData!B17)</f>
+        <f>IF(OldData!B17="","",MID(OldData!B17,2,9999))</f>
         <v/>
       </c>
       <c r="C17" s="54" t="str">
-        <f>IF(OldData!C17="","",OldData!C17)</f>
+        <f>IF(OldData!C17="","",MID(OldData!C17,2,9999))</f>
         <v/>
       </c>
       <c r="D17" s="32" t="str">
@@ -2463,7 +2510,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R17,'New Data'!$R$16:$R$115,0),CELL("colonne",P17)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R17,'New Data'!$R$16:$R$115,0),CELL("colonne",P17)-3)),IF(OldData!P17="","",OldData!P17))</f>
         <v/>
       </c>
-      <c r="R17" s="110" t="str">
+      <c r="R17" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2474,11 +2521,11 @@
         <v/>
       </c>
       <c r="B18" s="53" t="str">
-        <f>IF(OldData!B18="","",OldData!B18)</f>
+        <f>IF(OldData!B18="","",MID(OldData!B18,2,9999))</f>
         <v/>
       </c>
       <c r="C18" s="54" t="str">
-        <f>IF(OldData!C18="","",OldData!C18)</f>
+        <f>IF(OldData!C18="","",MID(OldData!C18,2,9999))</f>
         <v/>
       </c>
       <c r="D18" s="32" t="str">
@@ -2533,7 +2580,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R18,'New Data'!$R$16:$R$115,0),CELL("colonne",P18)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R18,'New Data'!$R$16:$R$115,0),CELL("colonne",P18)-3)),IF(OldData!P18="","",OldData!P18))</f>
         <v/>
       </c>
-      <c r="R18" s="110" t="str">
+      <c r="R18" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2544,11 +2591,11 @@
         <v/>
       </c>
       <c r="B19" s="53" t="str">
-        <f>IF(OldData!B19="","",OldData!B19)</f>
+        <f>IF(OldData!B19="","",MID(OldData!B19,2,9999))</f>
         <v/>
       </c>
       <c r="C19" s="54" t="str">
-        <f>IF(OldData!C19="","",OldData!C19)</f>
+        <f>IF(OldData!C19="","",MID(OldData!C19,2,9999))</f>
         <v/>
       </c>
       <c r="D19" s="32" t="str">
@@ -2603,7 +2650,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R19,'New Data'!$R$16:$R$115,0),CELL("colonne",P19)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R19,'New Data'!$R$16:$R$115,0),CELL("colonne",P19)-3)),IF(OldData!P19="","",OldData!P19))</f>
         <v/>
       </c>
-      <c r="R19" s="110" t="str">
+      <c r="R19" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2614,11 +2661,11 @@
         <v/>
       </c>
       <c r="B20" s="53" t="str">
-        <f>IF(OldData!B20="","",OldData!B20)</f>
+        <f>IF(OldData!B20="","",MID(OldData!B20,2,9999))</f>
         <v/>
       </c>
       <c r="C20" s="54" t="str">
-        <f>IF(OldData!C20="","",OldData!C20)</f>
+        <f>IF(OldData!C20="","",MID(OldData!C20,2,9999))</f>
         <v/>
       </c>
       <c r="D20" s="32" t="str">
@@ -2673,7 +2720,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R20,'New Data'!$R$16:$R$115,0),CELL("colonne",P20)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R20,'New Data'!$R$16:$R$115,0),CELL("colonne",P20)-3)),IF(OldData!P20="","",OldData!P20))</f>
         <v/>
       </c>
-      <c r="R20" s="110" t="str">
+      <c r="R20" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2684,11 +2731,11 @@
         <v/>
       </c>
       <c r="B21" s="53" t="str">
-        <f>IF(OldData!B21="","",OldData!B21)</f>
+        <f>IF(OldData!B21="","",MID(OldData!B21,2,9999))</f>
         <v/>
       </c>
       <c r="C21" s="54" t="str">
-        <f>IF(OldData!C21="","",OldData!C21)</f>
+        <f>IF(OldData!C21="","",MID(OldData!C21,2,9999))</f>
         <v/>
       </c>
       <c r="D21" s="32" t="str">
@@ -2743,7 +2790,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R21,'New Data'!$R$16:$R$115,0),CELL("colonne",P21)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R21,'New Data'!$R$16:$R$115,0),CELL("colonne",P21)-3)),IF(OldData!P21="","",OldData!P21))</f>
         <v/>
       </c>
-      <c r="R21" s="110" t="str">
+      <c r="R21" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2754,11 +2801,11 @@
         <v/>
       </c>
       <c r="B22" s="53" t="str">
-        <f>IF(OldData!B22="","",OldData!B22)</f>
+        <f>IF(OldData!B22="","",MID(OldData!B22,2,9999))</f>
         <v/>
       </c>
       <c r="C22" s="54" t="str">
-        <f>IF(OldData!C22="","",OldData!C22)</f>
+        <f>IF(OldData!C22="","",MID(OldData!C22,2,9999))</f>
         <v/>
       </c>
       <c r="D22" s="32" t="str">
@@ -2813,7 +2860,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R22,'New Data'!$R$16:$R$115,0),CELL("colonne",P22)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R22,'New Data'!$R$16:$R$115,0),CELL("colonne",P22)-3)),IF(OldData!P22="","",OldData!P22))</f>
         <v/>
       </c>
-      <c r="R22" s="110" t="str">
+      <c r="R22" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2824,11 +2871,11 @@
         <v/>
       </c>
       <c r="B23" s="53" t="str">
-        <f>IF(OldData!B23="","",OldData!B23)</f>
+        <f>IF(OldData!B23="","",MID(OldData!B23,2,9999))</f>
         <v/>
       </c>
       <c r="C23" s="54" t="str">
-        <f>IF(OldData!C23="","",OldData!C23)</f>
+        <f>IF(OldData!C23="","",MID(OldData!C23,2,9999))</f>
         <v/>
       </c>
       <c r="D23" s="32" t="str">
@@ -2883,7 +2930,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R23,'New Data'!$R$16:$R$115,0),CELL("colonne",P23)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R23,'New Data'!$R$16:$R$115,0),CELL("colonne",P23)-3)),IF(OldData!P23="","",OldData!P23))</f>
         <v/>
       </c>
-      <c r="R23" s="110" t="str">
+      <c r="R23" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2894,11 +2941,11 @@
         <v/>
       </c>
       <c r="B24" s="53" t="str">
-        <f>IF(OldData!B24="","",OldData!B24)</f>
+        <f>IF(OldData!B24="","",MID(OldData!B24,2,9999))</f>
         <v/>
       </c>
       <c r="C24" s="54" t="str">
-        <f>IF(OldData!C24="","",OldData!C24)</f>
+        <f>IF(OldData!C24="","",MID(OldData!C24,2,9999))</f>
         <v/>
       </c>
       <c r="D24" s="32" t="str">
@@ -2953,7 +3000,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R24,'New Data'!$R$16:$R$115,0),CELL("colonne",P24)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R24,'New Data'!$R$16:$R$115,0),CELL("colonne",P24)-3)),IF(OldData!P24="","",OldData!P24))</f>
         <v/>
       </c>
-      <c r="R24" s="110" t="str">
+      <c r="R24" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2964,11 +3011,11 @@
         <v/>
       </c>
       <c r="B25" s="53" t="str">
-        <f>IF(OldData!B25="","",OldData!B25)</f>
+        <f>IF(OldData!B25="","",MID(OldData!B25,2,9999))</f>
         <v/>
       </c>
       <c r="C25" s="54" t="str">
-        <f>IF(OldData!C25="","",OldData!C25)</f>
+        <f>IF(OldData!C25="","",MID(OldData!C25,2,9999))</f>
         <v/>
       </c>
       <c r="D25" s="32" t="str">
@@ -3023,7 +3070,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R25,'New Data'!$R$16:$R$115,0),CELL("colonne",P25)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R25,'New Data'!$R$16:$R$115,0),CELL("colonne",P25)-3)),IF(OldData!P25="","",OldData!P25))</f>
         <v/>
       </c>
-      <c r="R25" s="110" t="str">
+      <c r="R25" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3034,11 +3081,11 @@
         <v/>
       </c>
       <c r="B26" s="53" t="str">
-        <f>IF(OldData!B26="","",OldData!B26)</f>
+        <f>IF(OldData!B26="","",MID(OldData!B26,2,9999))</f>
         <v/>
       </c>
       <c r="C26" s="54" t="str">
-        <f>IF(OldData!C26="","",OldData!C26)</f>
+        <f>IF(OldData!C26="","",MID(OldData!C26,2,9999))</f>
         <v/>
       </c>
       <c r="D26" s="32" t="str">
@@ -3093,7 +3140,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R26,'New Data'!$R$16:$R$115,0),CELL("colonne",P26)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R26,'New Data'!$R$16:$R$115,0),CELL("colonne",P26)-3)),IF(OldData!P26="","",OldData!P26))</f>
         <v/>
       </c>
-      <c r="R26" s="110" t="str">
+      <c r="R26" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3104,11 +3151,11 @@
         <v/>
       </c>
       <c r="B27" s="53" t="str">
-        <f>IF(OldData!B27="","",OldData!B27)</f>
+        <f>IF(OldData!B27="","",MID(OldData!B27,2,9999))</f>
         <v/>
       </c>
       <c r="C27" s="54" t="str">
-        <f>IF(OldData!C27="","",OldData!C27)</f>
+        <f>IF(OldData!C27="","",MID(OldData!C27,2,9999))</f>
         <v/>
       </c>
       <c r="D27" s="32" t="str">
@@ -3163,7 +3210,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R27,'New Data'!$R$16:$R$115,0),CELL("colonne",P27)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R27,'New Data'!$R$16:$R$115,0),CELL("colonne",P27)-3)),IF(OldData!P27="","",OldData!P27))</f>
         <v/>
       </c>
-      <c r="R27" s="110" t="str">
+      <c r="R27" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3174,11 +3221,11 @@
         <v/>
       </c>
       <c r="B28" s="53" t="str">
-        <f>IF(OldData!B28="","",OldData!B28)</f>
+        <f>IF(OldData!B28="","",MID(OldData!B28,2,9999))</f>
         <v/>
       </c>
       <c r="C28" s="54" t="str">
-        <f>IF(OldData!C28="","",OldData!C28)</f>
+        <f>IF(OldData!C28="","",MID(OldData!C28,2,9999))</f>
         <v/>
       </c>
       <c r="D28" s="32" t="str">
@@ -3233,7 +3280,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R28,'New Data'!$R$16:$R$115,0),CELL("colonne",P28)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R28,'New Data'!$R$16:$R$115,0),CELL("colonne",P28)-3)),IF(OldData!P28="","",OldData!P28))</f>
         <v/>
       </c>
-      <c r="R28" s="110" t="str">
+      <c r="R28" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3244,11 +3291,11 @@
         <v/>
       </c>
       <c r="B29" s="53" t="str">
-        <f>IF(OldData!B29="","",OldData!B29)</f>
+        <f>IF(OldData!B29="","",MID(OldData!B29,2,9999))</f>
         <v/>
       </c>
       <c r="C29" s="54" t="str">
-        <f>IF(OldData!C29="","",OldData!C29)</f>
+        <f>IF(OldData!C29="","",MID(OldData!C29,2,9999))</f>
         <v/>
       </c>
       <c r="D29" s="32" t="str">
@@ -3303,7 +3350,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R29,'New Data'!$R$16:$R$115,0),CELL("colonne",P29)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R29,'New Data'!$R$16:$R$115,0),CELL("colonne",P29)-3)),IF(OldData!P29="","",OldData!P29))</f>
         <v/>
       </c>
-      <c r="R29" s="110" t="str">
+      <c r="R29" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3314,11 +3361,11 @@
         <v/>
       </c>
       <c r="B30" s="53" t="str">
-        <f>IF(OldData!B30="","",OldData!B30)</f>
+        <f>IF(OldData!B30="","",MID(OldData!B30,2,9999))</f>
         <v/>
       </c>
       <c r="C30" s="54" t="str">
-        <f>IF(OldData!C30="","",OldData!C30)</f>
+        <f>IF(OldData!C30="","",MID(OldData!C30,2,9999))</f>
         <v/>
       </c>
       <c r="D30" s="32" t="str">
@@ -3373,7 +3420,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R30,'New Data'!$R$16:$R$115,0),CELL("colonne",P30)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R30,'New Data'!$R$16:$R$115,0),CELL("colonne",P30)-3)),IF(OldData!P30="","",OldData!P30))</f>
         <v/>
       </c>
-      <c r="R30" s="110" t="str">
+      <c r="R30" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3384,11 +3431,11 @@
         <v/>
       </c>
       <c r="B31" s="53" t="str">
-        <f>IF(OldData!B31="","",OldData!B31)</f>
+        <f>IF(OldData!B31="","",MID(OldData!B31,2,9999))</f>
         <v/>
       </c>
       <c r="C31" s="54" t="str">
-        <f>IF(OldData!C31="","",OldData!C31)</f>
+        <f>IF(OldData!C31="","",MID(OldData!C31,2,9999))</f>
         <v/>
       </c>
       <c r="D31" s="32" t="str">
@@ -3443,7 +3490,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R31,'New Data'!$R$16:$R$115,0),CELL("colonne",P31)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R31,'New Data'!$R$16:$R$115,0),CELL("colonne",P31)-3)),IF(OldData!P31="","",OldData!P31))</f>
         <v/>
       </c>
-      <c r="R31" s="110" t="str">
+      <c r="R31" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3454,11 +3501,11 @@
         <v/>
       </c>
       <c r="B32" s="53" t="str">
-        <f>IF(OldData!B32="","",OldData!B32)</f>
+        <f>IF(OldData!B32="","",MID(OldData!B32,2,9999))</f>
         <v/>
       </c>
       <c r="C32" s="54" t="str">
-        <f>IF(OldData!C32="","",OldData!C32)</f>
+        <f>IF(OldData!C32="","",MID(OldData!C32,2,9999))</f>
         <v/>
       </c>
       <c r="D32" s="32" t="str">
@@ -3513,7 +3560,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R32,'New Data'!$R$16:$R$115,0),CELL("colonne",P32)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R32,'New Data'!$R$16:$R$115,0),CELL("colonne",P32)-3)),IF(OldData!P32="","",OldData!P32))</f>
         <v/>
       </c>
-      <c r="R32" s="110" t="str">
+      <c r="R32" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3524,11 +3571,11 @@
         <v/>
       </c>
       <c r="B33" s="53" t="str">
-        <f>IF(OldData!B33="","",OldData!B33)</f>
+        <f>IF(OldData!B33="","",MID(OldData!B33,2,9999))</f>
         <v/>
       </c>
       <c r="C33" s="54" t="str">
-        <f>IF(OldData!C33="","",OldData!C33)</f>
+        <f>IF(OldData!C33="","",MID(OldData!C33,2,9999))</f>
         <v/>
       </c>
       <c r="D33" s="32" t="str">
@@ -3583,7 +3630,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R33,'New Data'!$R$16:$R$115,0),CELL("colonne",P33)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R33,'New Data'!$R$16:$R$115,0),CELL("colonne",P33)-3)),IF(OldData!P33="","",OldData!P33))</f>
         <v/>
       </c>
-      <c r="R33" s="110" t="str">
+      <c r="R33" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3594,11 +3641,11 @@
         <v/>
       </c>
       <c r="B34" s="53" t="str">
-        <f>IF(OldData!B34="","",OldData!B34)</f>
+        <f>IF(OldData!B34="","",MID(OldData!B34,2,9999))</f>
         <v/>
       </c>
       <c r="C34" s="54" t="str">
-        <f>IF(OldData!C34="","",OldData!C34)</f>
+        <f>IF(OldData!C34="","",MID(OldData!C34,2,9999))</f>
         <v/>
       </c>
       <c r="D34" s="32" t="str">
@@ -3653,7 +3700,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R34,'New Data'!$R$16:$R$115,0),CELL("colonne",P34)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R34,'New Data'!$R$16:$R$115,0),CELL("colonne",P34)-3)),IF(OldData!P34="","",OldData!P34))</f>
         <v/>
       </c>
-      <c r="R34" s="110" t="str">
+      <c r="R34" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3664,11 +3711,11 @@
         <v/>
       </c>
       <c r="B35" s="53" t="str">
-        <f>IF(OldData!B35="","",OldData!B35)</f>
+        <f>IF(OldData!B35="","",MID(OldData!B35,2,9999))</f>
         <v/>
       </c>
       <c r="C35" s="54" t="str">
-        <f>IF(OldData!C35="","",OldData!C35)</f>
+        <f>IF(OldData!C35="","",MID(OldData!C35,2,9999))</f>
         <v/>
       </c>
       <c r="D35" s="32" t="str">
@@ -3723,7 +3770,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R35,'New Data'!$R$16:$R$115,0),CELL("colonne",P35)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R35,'New Data'!$R$16:$R$115,0),CELL("colonne",P35)-3)),IF(OldData!P35="","",OldData!P35))</f>
         <v/>
       </c>
-      <c r="R35" s="110" t="str">
+      <c r="R35" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3734,11 +3781,11 @@
         <v/>
       </c>
       <c r="B36" s="53" t="str">
-        <f>IF(OldData!B36="","",OldData!B36)</f>
+        <f>IF(OldData!B36="","",MID(OldData!B36,2,9999))</f>
         <v/>
       </c>
       <c r="C36" s="54" t="str">
-        <f>IF(OldData!C36="","",OldData!C36)</f>
+        <f>IF(OldData!C36="","",MID(OldData!C36,2,9999))</f>
         <v/>
       </c>
       <c r="D36" s="32" t="str">
@@ -3793,7 +3840,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R36,'New Data'!$R$16:$R$115,0),CELL("colonne",P36)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R36,'New Data'!$R$16:$R$115,0),CELL("colonne",P36)-3)),IF(OldData!P36="","",OldData!P36))</f>
         <v/>
       </c>
-      <c r="R36" s="110" t="str">
+      <c r="R36" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3804,11 +3851,11 @@
         <v/>
       </c>
       <c r="B37" s="53" t="str">
-        <f>IF(OldData!B37="","",OldData!B37)</f>
+        <f>IF(OldData!B37="","",MID(OldData!B37,2,9999))</f>
         <v/>
       </c>
       <c r="C37" s="54" t="str">
-        <f>IF(OldData!C37="","",OldData!C37)</f>
+        <f>IF(OldData!C37="","",MID(OldData!C37,2,9999))</f>
         <v/>
       </c>
       <c r="D37" s="32" t="str">
@@ -3863,7 +3910,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R37,'New Data'!$R$16:$R$115,0),CELL("colonne",P37)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R37,'New Data'!$R$16:$R$115,0),CELL("colonne",P37)-3)),IF(OldData!P37="","",OldData!P37))</f>
         <v/>
       </c>
-      <c r="R37" s="110" t="str">
+      <c r="R37" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3874,11 +3921,11 @@
         <v/>
       </c>
       <c r="B38" s="53" t="str">
-        <f>IF(OldData!B38="","",OldData!B38)</f>
+        <f>IF(OldData!B38="","",MID(OldData!B38,2,9999))</f>
         <v/>
       </c>
       <c r="C38" s="54" t="str">
-        <f>IF(OldData!C38="","",OldData!C38)</f>
+        <f>IF(OldData!C38="","",MID(OldData!C38,2,9999))</f>
         <v/>
       </c>
       <c r="D38" s="32" t="str">
@@ -3933,7 +3980,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R38,'New Data'!$R$16:$R$115,0),CELL("colonne",P38)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R38,'New Data'!$R$16:$R$115,0),CELL("colonne",P38)-3)),IF(OldData!P38="","",OldData!P38))</f>
         <v/>
       </c>
-      <c r="R38" s="110" t="str">
+      <c r="R38" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3944,11 +3991,11 @@
         <v/>
       </c>
       <c r="B39" s="53" t="str">
-        <f>IF(OldData!B39="","",OldData!B39)</f>
+        <f>IF(OldData!B39="","",MID(OldData!B39,2,9999))</f>
         <v/>
       </c>
       <c r="C39" s="54" t="str">
-        <f>IF(OldData!C39="","",OldData!C39)</f>
+        <f>IF(OldData!C39="","",MID(OldData!C39,2,9999))</f>
         <v/>
       </c>
       <c r="D39" s="32" t="str">
@@ -4003,7 +4050,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R39,'New Data'!$R$16:$R$115,0),CELL("colonne",P39)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R39,'New Data'!$R$16:$R$115,0),CELL("colonne",P39)-3)),IF(OldData!P39="","",OldData!P39))</f>
         <v/>
       </c>
-      <c r="R39" s="110" t="str">
+      <c r="R39" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4014,11 +4061,11 @@
         <v/>
       </c>
       <c r="B40" s="53" t="str">
-        <f>IF(OldData!B40="","",OldData!B40)</f>
+        <f>IF(OldData!B40="","",MID(OldData!B40,2,9999))</f>
         <v/>
       </c>
       <c r="C40" s="54" t="str">
-        <f>IF(OldData!C40="","",OldData!C40)</f>
+        <f>IF(OldData!C40="","",MID(OldData!C40,2,9999))</f>
         <v/>
       </c>
       <c r="D40" s="32" t="str">
@@ -4073,7 +4120,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R40,'New Data'!$R$16:$R$115,0),CELL("colonne",P40)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R40,'New Data'!$R$16:$R$115,0),CELL("colonne",P40)-3)),IF(OldData!P40="","",OldData!P40))</f>
         <v/>
       </c>
-      <c r="R40" s="110" t="str">
+      <c r="R40" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4084,11 +4131,11 @@
         <v/>
       </c>
       <c r="B41" s="53" t="str">
-        <f>IF(OldData!B41="","",OldData!B41)</f>
+        <f>IF(OldData!B41="","",MID(OldData!B41,2,9999))</f>
         <v/>
       </c>
       <c r="C41" s="54" t="str">
-        <f>IF(OldData!C41="","",OldData!C41)</f>
+        <f>IF(OldData!C41="","",MID(OldData!C41,2,9999))</f>
         <v/>
       </c>
       <c r="D41" s="32" t="str">
@@ -4143,7 +4190,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R41,'New Data'!$R$16:$R$115,0),CELL("colonne",P41)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R41,'New Data'!$R$16:$R$115,0),CELL("colonne",P41)-3)),IF(OldData!P41="","",OldData!P41))</f>
         <v/>
       </c>
-      <c r="R41" s="110" t="str">
+      <c r="R41" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4154,11 +4201,11 @@
         <v/>
       </c>
       <c r="B42" s="53" t="str">
-        <f>IF(OldData!B42="","",OldData!B42)</f>
+        <f>IF(OldData!B42="","",MID(OldData!B42,2,9999))</f>
         <v/>
       </c>
       <c r="C42" s="54" t="str">
-        <f>IF(OldData!C42="","",OldData!C42)</f>
+        <f>IF(OldData!C42="","",MID(OldData!C42,2,9999))</f>
         <v/>
       </c>
       <c r="D42" s="32" t="str">
@@ -4213,7 +4260,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R42,'New Data'!$R$16:$R$115,0),CELL("colonne",P42)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R42,'New Data'!$R$16:$R$115,0),CELL("colonne",P42)-3)),IF(OldData!P42="","",OldData!P42))</f>
         <v/>
       </c>
-      <c r="R42" s="110" t="str">
+      <c r="R42" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4224,11 +4271,11 @@
         <v/>
       </c>
       <c r="B43" s="53" t="str">
-        <f>IF(OldData!B43="","",OldData!B43)</f>
+        <f>IF(OldData!B43="","",MID(OldData!B43,2,9999))</f>
         <v/>
       </c>
       <c r="C43" s="54" t="str">
-        <f>IF(OldData!C43="","",OldData!C43)</f>
+        <f>IF(OldData!C43="","",MID(OldData!C43,2,9999))</f>
         <v/>
       </c>
       <c r="D43" s="32" t="str">
@@ -4283,7 +4330,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R43,'New Data'!$R$16:$R$115,0),CELL("colonne",P43)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R43,'New Data'!$R$16:$R$115,0),CELL("colonne",P43)-3)),IF(OldData!P43="","",OldData!P43))</f>
         <v/>
       </c>
-      <c r="R43" s="110" t="str">
+      <c r="R43" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4294,11 +4341,11 @@
         <v/>
       </c>
       <c r="B44" s="53" t="str">
-        <f>IF(OldData!B44="","",OldData!B44)</f>
+        <f>IF(OldData!B44="","",MID(OldData!B44,2,9999))</f>
         <v/>
       </c>
       <c r="C44" s="54" t="str">
-        <f>IF(OldData!C44="","",OldData!C44)</f>
+        <f>IF(OldData!C44="","",MID(OldData!C44,2,9999))</f>
         <v/>
       </c>
       <c r="D44" s="32" t="str">
@@ -4353,7 +4400,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R44,'New Data'!$R$16:$R$115,0),CELL("colonne",P44)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R44,'New Data'!$R$16:$R$115,0),CELL("colonne",P44)-3)),IF(OldData!P44="","",OldData!P44))</f>
         <v/>
       </c>
-      <c r="R44" s="110" t="str">
+      <c r="R44" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4364,11 +4411,11 @@
         <v/>
       </c>
       <c r="B45" s="53" t="str">
-        <f>IF(OldData!B45="","",OldData!B45)</f>
+        <f>IF(OldData!B45="","",MID(OldData!B45,2,9999))</f>
         <v/>
       </c>
       <c r="C45" s="54" t="str">
-        <f>IF(OldData!C45="","",OldData!C45)</f>
+        <f>IF(OldData!C45="","",MID(OldData!C45,2,9999))</f>
         <v/>
       </c>
       <c r="D45" s="32" t="str">
@@ -4423,7 +4470,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R45,'New Data'!$R$16:$R$115,0),CELL("colonne",P45)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R45,'New Data'!$R$16:$R$115,0),CELL("colonne",P45)-3)),IF(OldData!P45="","",OldData!P45))</f>
         <v/>
       </c>
-      <c r="R45" s="110" t="str">
+      <c r="R45" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4434,11 +4481,11 @@
         <v/>
       </c>
       <c r="B46" s="53" t="str">
-        <f>IF(OldData!B46="","",OldData!B46)</f>
+        <f>IF(OldData!B46="","",MID(OldData!B46,2,9999))</f>
         <v/>
       </c>
       <c r="C46" s="54" t="str">
-        <f>IF(OldData!C46="","",OldData!C46)</f>
+        <f>IF(OldData!C46="","",MID(OldData!C46,2,9999))</f>
         <v/>
       </c>
       <c r="D46" s="32" t="str">
@@ -4493,7 +4540,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R46,'New Data'!$R$16:$R$115,0),CELL("colonne",P46)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R46,'New Data'!$R$16:$R$115,0),CELL("colonne",P46)-3)),IF(OldData!P46="","",OldData!P46))</f>
         <v/>
       </c>
-      <c r="R46" s="110" t="str">
+      <c r="R46" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4504,11 +4551,11 @@
         <v/>
       </c>
       <c r="B47" s="53" t="str">
-        <f>IF(OldData!B47="","",OldData!B47)</f>
+        <f>IF(OldData!B47="","",MID(OldData!B47,2,9999))</f>
         <v/>
       </c>
       <c r="C47" s="54" t="str">
-        <f>IF(OldData!C47="","",OldData!C47)</f>
+        <f>IF(OldData!C47="","",MID(OldData!C47,2,9999))</f>
         <v/>
       </c>
       <c r="D47" s="32" t="str">
@@ -4563,7 +4610,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R47,'New Data'!$R$16:$R$115,0),CELL("colonne",P47)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R47,'New Data'!$R$16:$R$115,0),CELL("colonne",P47)-3)),IF(OldData!P47="","",OldData!P47))</f>
         <v/>
       </c>
-      <c r="R47" s="110" t="str">
+      <c r="R47" s="109" t="str">
         <f t="shared" ref="R47:R48" si="1">B47&amp;C47</f>
         <v/>
       </c>
@@ -4574,11 +4621,11 @@
         <v/>
       </c>
       <c r="B48" s="53" t="str">
-        <f>IF(OldData!B48="","",OldData!B48)</f>
+        <f>IF(OldData!B48="","",MID(OldData!B48,2,9999))</f>
         <v/>
       </c>
       <c r="C48" s="54" t="str">
-        <f>IF(OldData!C48="","",OldData!C48)</f>
+        <f>IF(OldData!C48="","",MID(OldData!C48,2,9999))</f>
         <v/>
       </c>
       <c r="D48" s="32" t="str">
@@ -4633,7 +4680,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R48,'New Data'!$R$16:$R$115,0),CELL("colonne",P48)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R48,'New Data'!$R$16:$R$115,0),CELL("colonne",P48)-3)),IF(OldData!P48="","",OldData!P48))</f>
         <v/>
       </c>
-      <c r="R48" s="110" t="str">
+      <c r="R48" s="109" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4644,11 +4691,11 @@
         <v/>
       </c>
       <c r="B49" s="53" t="str">
-        <f>IF(OldData!B49="","",OldData!B49)</f>
+        <f>IF(OldData!B49="","",MID(OldData!B49,2,9999))</f>
         <v/>
       </c>
       <c r="C49" s="54" t="str">
-        <f>IF(OldData!C49="","",OldData!C49)</f>
+        <f>IF(OldData!C49="","",MID(OldData!C49,2,9999))</f>
         <v/>
       </c>
       <c r="D49" s="32" t="str">
@@ -4714,11 +4761,11 @@
         <v/>
       </c>
       <c r="B50" s="53" t="str">
-        <f>IF(OldData!B50="","",OldData!B50)</f>
+        <f>IF(OldData!B50="","",MID(OldData!B50,2,9999))</f>
         <v/>
       </c>
       <c r="C50" s="54" t="str">
-        <f>IF(OldData!C50="","",OldData!C50)</f>
+        <f>IF(OldData!C50="","",MID(OldData!C50,2,9999))</f>
         <v/>
       </c>
       <c r="D50" s="32" t="str">
@@ -4773,7 +4820,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R50,'New Data'!$R$16:$R$115,0),CELL("colonne",P50)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R50,'New Data'!$R$16:$R$115,0),CELL("colonne",P50)-3)),IF(OldData!P50="","",OldData!P50))</f>
         <v/>
       </c>
-      <c r="R50" s="110" t="str">
+      <c r="R50" s="109" t="str">
         <f t="shared" ref="R50:R113" si="2">B50&amp;C50</f>
         <v/>
       </c>
@@ -4784,11 +4831,11 @@
         <v/>
       </c>
       <c r="B51" s="53" t="str">
-        <f>IF(OldData!B51="","",OldData!B51)</f>
+        <f>IF(OldData!B51="","",MID(OldData!B51,2,9999))</f>
         <v/>
       </c>
       <c r="C51" s="54" t="str">
-        <f>IF(OldData!C51="","",OldData!C51)</f>
+        <f>IF(OldData!C51="","",MID(OldData!C51,2,9999))</f>
         <v/>
       </c>
       <c r="D51" s="32" t="str">
@@ -4843,7 +4890,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R51,'New Data'!$R$16:$R$115,0),CELL("colonne",P51)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R51,'New Data'!$R$16:$R$115,0),CELL("colonne",P51)-3)),IF(OldData!P51="","",OldData!P51))</f>
         <v/>
       </c>
-      <c r="R51" s="110" t="str">
+      <c r="R51" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4854,11 +4901,11 @@
         <v/>
       </c>
       <c r="B52" s="53" t="str">
-        <f>IF(OldData!B52="","",OldData!B52)</f>
+        <f>IF(OldData!B52="","",MID(OldData!B52,2,9999))</f>
         <v/>
       </c>
       <c r="C52" s="54" t="str">
-        <f>IF(OldData!C52="","",OldData!C52)</f>
+        <f>IF(OldData!C52="","",MID(OldData!C52,2,9999))</f>
         <v/>
       </c>
       <c r="D52" s="32" t="str">
@@ -4913,7 +4960,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R52,'New Data'!$R$16:$R$115,0),CELL("colonne",P52)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R52,'New Data'!$R$16:$R$115,0),CELL("colonne",P52)-3)),IF(OldData!P52="","",OldData!P52))</f>
         <v/>
       </c>
-      <c r="R52" s="110" t="str">
+      <c r="R52" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4924,11 +4971,11 @@
         <v/>
       </c>
       <c r="B53" s="53" t="str">
-        <f>IF(OldData!B53="","",OldData!B53)</f>
+        <f>IF(OldData!B53="","",MID(OldData!B53,2,9999))</f>
         <v/>
       </c>
       <c r="C53" s="54" t="str">
-        <f>IF(OldData!C53="","",OldData!C53)</f>
+        <f>IF(OldData!C53="","",MID(OldData!C53,2,9999))</f>
         <v/>
       </c>
       <c r="D53" s="32" t="str">
@@ -4983,7 +5030,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R53,'New Data'!$R$16:$R$115,0),CELL("colonne",P53)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R53,'New Data'!$R$16:$R$115,0),CELL("colonne",P53)-3)),IF(OldData!P53="","",OldData!P53))</f>
         <v/>
       </c>
-      <c r="R53" s="110" t="str">
+      <c r="R53" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4994,11 +5041,11 @@
         <v/>
       </c>
       <c r="B54" s="53" t="str">
-        <f>IF(OldData!B54="","",OldData!B54)</f>
+        <f>IF(OldData!B54="","",MID(OldData!B54,2,9999))</f>
         <v/>
       </c>
       <c r="C54" s="54" t="str">
-        <f>IF(OldData!C54="","",OldData!C54)</f>
+        <f>IF(OldData!C54="","",MID(OldData!C54,2,9999))</f>
         <v/>
       </c>
       <c r="D54" s="32" t="str">
@@ -5053,7 +5100,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R54,'New Data'!$R$16:$R$115,0),CELL("colonne",P54)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R54,'New Data'!$R$16:$R$115,0),CELL("colonne",P54)-3)),IF(OldData!P54="","",OldData!P54))</f>
         <v/>
       </c>
-      <c r="R54" s="110" t="str">
+      <c r="R54" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5064,11 +5111,11 @@
         <v/>
       </c>
       <c r="B55" s="53" t="str">
-        <f>IF(OldData!B55="","",OldData!B55)</f>
+        <f>IF(OldData!B55="","",MID(OldData!B55,2,9999))</f>
         <v/>
       </c>
       <c r="C55" s="54" t="str">
-        <f>IF(OldData!C55="","",OldData!C55)</f>
+        <f>IF(OldData!C55="","",MID(OldData!C55,2,9999))</f>
         <v/>
       </c>
       <c r="D55" s="32" t="str">
@@ -5123,7 +5170,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R55,'New Data'!$R$16:$R$115,0),CELL("colonne",P55)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R55,'New Data'!$R$16:$R$115,0),CELL("colonne",P55)-3)),IF(OldData!P55="","",OldData!P55))</f>
         <v/>
       </c>
-      <c r="R55" s="110" t="str">
+      <c r="R55" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5134,11 +5181,11 @@
         <v/>
       </c>
       <c r="B56" s="53" t="str">
-        <f>IF(OldData!B56="","",OldData!B56)</f>
+        <f>IF(OldData!B56="","",MID(OldData!B56,2,9999))</f>
         <v/>
       </c>
       <c r="C56" s="54" t="str">
-        <f>IF(OldData!C56="","",OldData!C56)</f>
+        <f>IF(OldData!C56="","",MID(OldData!C56,2,9999))</f>
         <v/>
       </c>
       <c r="D56" s="32" t="str">
@@ -5193,7 +5240,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R56,'New Data'!$R$16:$R$115,0),CELL("colonne",P56)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R56,'New Data'!$R$16:$R$115,0),CELL("colonne",P56)-3)),IF(OldData!P56="","",OldData!P56))</f>
         <v/>
       </c>
-      <c r="R56" s="110" t="str">
+      <c r="R56" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5204,11 +5251,11 @@
         <v/>
       </c>
       <c r="B57" s="53" t="str">
-        <f>IF(OldData!B57="","",OldData!B57)</f>
+        <f>IF(OldData!B57="","",MID(OldData!B57,2,9999))</f>
         <v/>
       </c>
       <c r="C57" s="54" t="str">
-        <f>IF(OldData!C57="","",OldData!C57)</f>
+        <f>IF(OldData!C57="","",MID(OldData!C57,2,9999))</f>
         <v/>
       </c>
       <c r="D57" s="32" t="str">
@@ -5263,7 +5310,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R57,'New Data'!$R$16:$R$115,0),CELL("colonne",P57)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R57,'New Data'!$R$16:$R$115,0),CELL("colonne",P57)-3)),IF(OldData!P57="","",OldData!P57))</f>
         <v/>
       </c>
-      <c r="R57" s="110" t="str">
+      <c r="R57" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5274,11 +5321,11 @@
         <v/>
       </c>
       <c r="B58" s="53" t="str">
-        <f>IF(OldData!B58="","",OldData!B58)</f>
+        <f>IF(OldData!B58="","",MID(OldData!B58,2,9999))</f>
         <v/>
       </c>
       <c r="C58" s="54" t="str">
-        <f>IF(OldData!C58="","",OldData!C58)</f>
+        <f>IF(OldData!C58="","",MID(OldData!C58,2,9999))</f>
         <v/>
       </c>
       <c r="D58" s="32" t="str">
@@ -5333,7 +5380,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R58,'New Data'!$R$16:$R$115,0),CELL("colonne",P58)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R58,'New Data'!$R$16:$R$115,0),CELL("colonne",P58)-3)),IF(OldData!P58="","",OldData!P58))</f>
         <v/>
       </c>
-      <c r="R58" s="110" t="str">
+      <c r="R58" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5344,11 +5391,11 @@
         <v/>
       </c>
       <c r="B59" s="53" t="str">
-        <f>IF(OldData!B59="","",OldData!B59)</f>
+        <f>IF(OldData!B59="","",MID(OldData!B59,2,9999))</f>
         <v/>
       </c>
       <c r="C59" s="54" t="str">
-        <f>IF(OldData!C59="","",OldData!C59)</f>
+        <f>IF(OldData!C59="","",MID(OldData!C59,2,9999))</f>
         <v/>
       </c>
       <c r="D59" s="32" t="str">
@@ -5403,7 +5450,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R59,'New Data'!$R$16:$R$115,0),CELL("colonne",P59)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R59,'New Data'!$R$16:$R$115,0),CELL("colonne",P59)-3)),IF(OldData!P59="","",OldData!P59))</f>
         <v/>
       </c>
-      <c r="R59" s="110" t="str">
+      <c r="R59" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5414,11 +5461,11 @@
         <v/>
       </c>
       <c r="B60" s="53" t="str">
-        <f>IF(OldData!B60="","",OldData!B60)</f>
+        <f>IF(OldData!B60="","",MID(OldData!B60,2,9999))</f>
         <v/>
       </c>
       <c r="C60" s="54" t="str">
-        <f>IF(OldData!C60="","",OldData!C60)</f>
+        <f>IF(OldData!C60="","",MID(OldData!C60,2,9999))</f>
         <v/>
       </c>
       <c r="D60" s="32" t="str">
@@ -5473,7 +5520,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R60,'New Data'!$R$16:$R$115,0),CELL("colonne",P60)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R60,'New Data'!$R$16:$R$115,0),CELL("colonne",P60)-3)),IF(OldData!P60="","",OldData!P60))</f>
         <v/>
       </c>
-      <c r="R60" s="110" t="str">
+      <c r="R60" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5484,11 +5531,11 @@
         <v/>
       </c>
       <c r="B61" s="53" t="str">
-        <f>IF(OldData!B61="","",OldData!B61)</f>
+        <f>IF(OldData!B61="","",MID(OldData!B61,2,9999))</f>
         <v/>
       </c>
       <c r="C61" s="54" t="str">
-        <f>IF(OldData!C61="","",OldData!C61)</f>
+        <f>IF(OldData!C61="","",MID(OldData!C61,2,9999))</f>
         <v/>
       </c>
       <c r="D61" s="32" t="str">
@@ -5543,7 +5590,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R61,'New Data'!$R$16:$R$115,0),CELL("colonne",P61)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R61,'New Data'!$R$16:$R$115,0),CELL("colonne",P61)-3)),IF(OldData!P61="","",OldData!P61))</f>
         <v/>
       </c>
-      <c r="R61" s="110" t="str">
+      <c r="R61" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5554,11 +5601,11 @@
         <v/>
       </c>
       <c r="B62" s="53" t="str">
-        <f>IF(OldData!B62="","",OldData!B62)</f>
+        <f>IF(OldData!B62="","",MID(OldData!B62,2,9999))</f>
         <v/>
       </c>
       <c r="C62" s="54" t="str">
-        <f>IF(OldData!C62="","",OldData!C62)</f>
+        <f>IF(OldData!C62="","",MID(OldData!C62,2,9999))</f>
         <v/>
       </c>
       <c r="D62" s="32" t="str">
@@ -5613,7 +5660,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R62,'New Data'!$R$16:$R$115,0),CELL("colonne",P62)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R62,'New Data'!$R$16:$R$115,0),CELL("colonne",P62)-3)),IF(OldData!P62="","",OldData!P62))</f>
         <v/>
       </c>
-      <c r="R62" s="110" t="str">
+      <c r="R62" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5624,11 +5671,11 @@
         <v/>
       </c>
       <c r="B63" s="53" t="str">
-        <f>IF(OldData!B63="","",OldData!B63)</f>
+        <f>IF(OldData!B63="","",MID(OldData!B63,2,9999))</f>
         <v/>
       </c>
       <c r="C63" s="54" t="str">
-        <f>IF(OldData!C63="","",OldData!C63)</f>
+        <f>IF(OldData!C63="","",MID(OldData!C63,2,9999))</f>
         <v/>
       </c>
       <c r="D63" s="32" t="str">
@@ -5683,7 +5730,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R63,'New Data'!$R$16:$R$115,0),CELL("colonne",P63)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R63,'New Data'!$R$16:$R$115,0),CELL("colonne",P63)-3)),IF(OldData!P63="","",OldData!P63))</f>
         <v/>
       </c>
-      <c r="R63" s="110" t="str">
+      <c r="R63" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5694,11 +5741,11 @@
         <v/>
       </c>
       <c r="B64" s="53" t="str">
-        <f>IF(OldData!B64="","",OldData!B64)</f>
+        <f>IF(OldData!B64="","",MID(OldData!B64,2,9999))</f>
         <v/>
       </c>
       <c r="C64" s="54" t="str">
-        <f>IF(OldData!C64="","",OldData!C64)</f>
+        <f>IF(OldData!C64="","",MID(OldData!C64,2,9999))</f>
         <v/>
       </c>
       <c r="D64" s="32" t="str">
@@ -5753,7 +5800,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R64,'New Data'!$R$16:$R$115,0),CELL("colonne",P64)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R64,'New Data'!$R$16:$R$115,0),CELL("colonne",P64)-3)),IF(OldData!P64="","",OldData!P64))</f>
         <v/>
       </c>
-      <c r="R64" s="110" t="str">
+      <c r="R64" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5764,11 +5811,11 @@
         <v/>
       </c>
       <c r="B65" s="53" t="str">
-        <f>IF(OldData!B65="","",OldData!B65)</f>
+        <f>IF(OldData!B65="","",MID(OldData!B65,2,9999))</f>
         <v/>
       </c>
       <c r="C65" s="54" t="str">
-        <f>IF(OldData!C65="","",OldData!C65)</f>
+        <f>IF(OldData!C65="","",MID(OldData!C65,2,9999))</f>
         <v/>
       </c>
       <c r="D65" s="32" t="str">
@@ -5823,7 +5870,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R65,'New Data'!$R$16:$R$115,0),CELL("colonne",P65)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R65,'New Data'!$R$16:$R$115,0),CELL("colonne",P65)-3)),IF(OldData!P65="","",OldData!P65))</f>
         <v/>
       </c>
-      <c r="R65" s="110" t="str">
+      <c r="R65" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5834,11 +5881,11 @@
         <v/>
       </c>
       <c r="B66" s="53" t="str">
-        <f>IF(OldData!B66="","",OldData!B66)</f>
+        <f>IF(OldData!B66="","",MID(OldData!B66,2,9999))</f>
         <v/>
       </c>
       <c r="C66" s="54" t="str">
-        <f>IF(OldData!C66="","",OldData!C66)</f>
+        <f>IF(OldData!C66="","",MID(OldData!C66,2,9999))</f>
         <v/>
       </c>
       <c r="D66" s="32" t="str">
@@ -5893,7 +5940,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R66,'New Data'!$R$16:$R$115,0),CELL("colonne",P66)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R66,'New Data'!$R$16:$R$115,0),CELL("colonne",P66)-3)),IF(OldData!P66="","",OldData!P66))</f>
         <v/>
       </c>
-      <c r="R66" s="110" t="str">
+      <c r="R66" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5904,11 +5951,11 @@
         <v/>
       </c>
       <c r="B67" s="53" t="str">
-        <f>IF(OldData!B67="","",OldData!B67)</f>
+        <f>IF(OldData!B67="","",MID(OldData!B67,2,9999))</f>
         <v/>
       </c>
       <c r="C67" s="54" t="str">
-        <f>IF(OldData!C67="","",OldData!C67)</f>
+        <f>IF(OldData!C67="","",MID(OldData!C67,2,9999))</f>
         <v/>
       </c>
       <c r="D67" s="32" t="str">
@@ -5963,7 +6010,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R67,'New Data'!$R$16:$R$115,0),CELL("colonne",P67)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R67,'New Data'!$R$16:$R$115,0),CELL("colonne",P67)-3)),IF(OldData!P67="","",OldData!P67))</f>
         <v/>
       </c>
-      <c r="R67" s="110" t="str">
+      <c r="R67" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -5974,11 +6021,11 @@
         <v/>
       </c>
       <c r="B68" s="53" t="str">
-        <f>IF(OldData!B68="","",OldData!B68)</f>
+        <f>IF(OldData!B68="","",MID(OldData!B68,2,9999))</f>
         <v/>
       </c>
       <c r="C68" s="54" t="str">
-        <f>IF(OldData!C68="","",OldData!C68)</f>
+        <f>IF(OldData!C68="","",MID(OldData!C68,2,9999))</f>
         <v/>
       </c>
       <c r="D68" s="32" t="str">
@@ -6033,7 +6080,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R68,'New Data'!$R$16:$R$115,0),CELL("colonne",P68)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R68,'New Data'!$R$16:$R$115,0),CELL("colonne",P68)-3)),IF(OldData!P68="","",OldData!P68))</f>
         <v/>
       </c>
-      <c r="R68" s="110" t="str">
+      <c r="R68" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6044,11 +6091,11 @@
         <v/>
       </c>
       <c r="B69" s="53" t="str">
-        <f>IF(OldData!B69="","",OldData!B69)</f>
+        <f>IF(OldData!B69="","",MID(OldData!B69,2,9999))</f>
         <v/>
       </c>
       <c r="C69" s="54" t="str">
-        <f>IF(OldData!C69="","",OldData!C69)</f>
+        <f>IF(OldData!C69="","",MID(OldData!C69,2,9999))</f>
         <v/>
       </c>
       <c r="D69" s="32" t="str">
@@ -6103,7 +6150,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R69,'New Data'!$R$16:$R$115,0),CELL("colonne",P69)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R69,'New Data'!$R$16:$R$115,0),CELL("colonne",P69)-3)),IF(OldData!P69="","",OldData!P69))</f>
         <v/>
       </c>
-      <c r="R69" s="110" t="str">
+      <c r="R69" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6114,11 +6161,11 @@
         <v/>
       </c>
       <c r="B70" s="53" t="str">
-        <f>IF(OldData!B70="","",OldData!B70)</f>
+        <f>IF(OldData!B70="","",MID(OldData!B70,2,9999))</f>
         <v/>
       </c>
       <c r="C70" s="54" t="str">
-        <f>IF(OldData!C70="","",OldData!C70)</f>
+        <f>IF(OldData!C70="","",MID(OldData!C70,2,9999))</f>
         <v/>
       </c>
       <c r="D70" s="32" t="str">
@@ -6173,7 +6220,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R70,'New Data'!$R$16:$R$115,0),CELL("colonne",P70)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R70,'New Data'!$R$16:$R$115,0),CELL("colonne",P70)-3)),IF(OldData!P70="","",OldData!P70))</f>
         <v/>
       </c>
-      <c r="R70" s="110" t="str">
+      <c r="R70" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6184,11 +6231,11 @@
         <v/>
       </c>
       <c r="B71" s="53" t="str">
-        <f>IF(OldData!B71="","",OldData!B71)</f>
+        <f>IF(OldData!B71="","",MID(OldData!B71,2,9999))</f>
         <v/>
       </c>
       <c r="C71" s="54" t="str">
-        <f>IF(OldData!C71="","",OldData!C71)</f>
+        <f>IF(OldData!C71="","",MID(OldData!C71,2,9999))</f>
         <v/>
       </c>
       <c r="D71" s="32" t="str">
@@ -6243,7 +6290,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R71,'New Data'!$R$16:$R$115,0),CELL("colonne",P71)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R71,'New Data'!$R$16:$R$115,0),CELL("colonne",P71)-3)),IF(OldData!P71="","",OldData!P71))</f>
         <v/>
       </c>
-      <c r="R71" s="110" t="str">
+      <c r="R71" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6254,11 +6301,11 @@
         <v/>
       </c>
       <c r="B72" s="53" t="str">
-        <f>IF(OldData!B72="","",OldData!B72)</f>
+        <f>IF(OldData!B72="","",MID(OldData!B72,2,9999))</f>
         <v/>
       </c>
       <c r="C72" s="54" t="str">
-        <f>IF(OldData!C72="","",OldData!C72)</f>
+        <f>IF(OldData!C72="","",MID(OldData!C72,2,9999))</f>
         <v/>
       </c>
       <c r="D72" s="32" t="str">
@@ -6313,7 +6360,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R72,'New Data'!$R$16:$R$115,0),CELL("colonne",P72)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R72,'New Data'!$R$16:$R$115,0),CELL("colonne",P72)-3)),IF(OldData!P72="","",OldData!P72))</f>
         <v/>
       </c>
-      <c r="R72" s="110" t="str">
+      <c r="R72" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6324,11 +6371,11 @@
         <v/>
       </c>
       <c r="B73" s="53" t="str">
-        <f>IF(OldData!B73="","",OldData!B73)</f>
+        <f>IF(OldData!B73="","",MID(OldData!B73,2,9999))</f>
         <v/>
       </c>
       <c r="C73" s="54" t="str">
-        <f>IF(OldData!C73="","",OldData!C73)</f>
+        <f>IF(OldData!C73="","",MID(OldData!C73,2,9999))</f>
         <v/>
       </c>
       <c r="D73" s="32" t="str">
@@ -6383,7 +6430,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R73,'New Data'!$R$16:$R$115,0),CELL("colonne",P73)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R73,'New Data'!$R$16:$R$115,0),CELL("colonne",P73)-3)),IF(OldData!P73="","",OldData!P73))</f>
         <v/>
       </c>
-      <c r="R73" s="110" t="str">
+      <c r="R73" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6394,11 +6441,11 @@
         <v/>
       </c>
       <c r="B74" s="53" t="str">
-        <f>IF(OldData!B74="","",OldData!B74)</f>
+        <f>IF(OldData!B74="","",MID(OldData!B74,2,9999))</f>
         <v/>
       </c>
       <c r="C74" s="54" t="str">
-        <f>IF(OldData!C74="","",OldData!C74)</f>
+        <f>IF(OldData!C74="","",MID(OldData!C74,2,9999))</f>
         <v/>
       </c>
       <c r="D74" s="32" t="str">
@@ -6453,7 +6500,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R74,'New Data'!$R$16:$R$115,0),CELL("colonne",P74)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R74,'New Data'!$R$16:$R$115,0),CELL("colonne",P74)-3)),IF(OldData!P74="","",OldData!P74))</f>
         <v/>
       </c>
-      <c r="R74" s="110" t="str">
+      <c r="R74" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6464,11 +6511,11 @@
         <v/>
       </c>
       <c r="B75" s="53" t="str">
-        <f>IF(OldData!B75="","",OldData!B75)</f>
+        <f>IF(OldData!B75="","",MID(OldData!B75,2,9999))</f>
         <v/>
       </c>
       <c r="C75" s="54" t="str">
-        <f>IF(OldData!C75="","",OldData!C75)</f>
+        <f>IF(OldData!C75="","",MID(OldData!C75,2,9999))</f>
         <v/>
       </c>
       <c r="D75" s="32" t="str">
@@ -6523,7 +6570,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R75,'New Data'!$R$16:$R$115,0),CELL("colonne",P75)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R75,'New Data'!$R$16:$R$115,0),CELL("colonne",P75)-3)),IF(OldData!P75="","",OldData!P75))</f>
         <v/>
       </c>
-      <c r="R75" s="110" t="str">
+      <c r="R75" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6534,11 +6581,11 @@
         <v/>
       </c>
       <c r="B76" s="53" t="str">
-        <f>IF(OldData!B76="","",OldData!B76)</f>
+        <f>IF(OldData!B76="","",MID(OldData!B76,2,9999))</f>
         <v/>
       </c>
       <c r="C76" s="54" t="str">
-        <f>IF(OldData!C76="","",OldData!C76)</f>
+        <f>IF(OldData!C76="","",MID(OldData!C76,2,9999))</f>
         <v/>
       </c>
       <c r="D76" s="32" t="str">
@@ -6593,7 +6640,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R76,'New Data'!$R$16:$R$115,0),CELL("colonne",P76)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R76,'New Data'!$R$16:$R$115,0),CELL("colonne",P76)-3)),IF(OldData!P76="","",OldData!P76))</f>
         <v/>
       </c>
-      <c r="R76" s="110" t="str">
+      <c r="R76" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6604,11 +6651,11 @@
         <v/>
       </c>
       <c r="B77" s="53" t="str">
-        <f>IF(OldData!B77="","",OldData!B77)</f>
+        <f>IF(OldData!B77="","",MID(OldData!B77,2,9999))</f>
         <v/>
       </c>
       <c r="C77" s="54" t="str">
-        <f>IF(OldData!C77="","",OldData!C77)</f>
+        <f>IF(OldData!C77="","",MID(OldData!C77,2,9999))</f>
         <v/>
       </c>
       <c r="D77" s="32" t="str">
@@ -6663,7 +6710,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R77,'New Data'!$R$16:$R$115,0),CELL("colonne",P77)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R77,'New Data'!$R$16:$R$115,0),CELL("colonne",P77)-3)),IF(OldData!P77="","",OldData!P77))</f>
         <v/>
       </c>
-      <c r="R77" s="110" t="str">
+      <c r="R77" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6674,11 +6721,11 @@
         <v/>
       </c>
       <c r="B78" s="53" t="str">
-        <f>IF(OldData!B78="","",OldData!B78)</f>
+        <f>IF(OldData!B78="","",MID(OldData!B78,2,9999))</f>
         <v/>
       </c>
       <c r="C78" s="54" t="str">
-        <f>IF(OldData!C78="","",OldData!C78)</f>
+        <f>IF(OldData!C78="","",MID(OldData!C78,2,9999))</f>
         <v/>
       </c>
       <c r="D78" s="32" t="str">
@@ -6733,7 +6780,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R78,'New Data'!$R$16:$R$115,0),CELL("colonne",P78)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R78,'New Data'!$R$16:$R$115,0),CELL("colonne",P78)-3)),IF(OldData!P78="","",OldData!P78))</f>
         <v/>
       </c>
-      <c r="R78" s="110" t="str">
+      <c r="R78" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6744,11 +6791,11 @@
         <v/>
       </c>
       <c r="B79" s="53" t="str">
-        <f>IF(OldData!B79="","",OldData!B79)</f>
+        <f>IF(OldData!B79="","",MID(OldData!B79,2,9999))</f>
         <v/>
       </c>
       <c r="C79" s="54" t="str">
-        <f>IF(OldData!C79="","",OldData!C79)</f>
+        <f>IF(OldData!C79="","",MID(OldData!C79,2,9999))</f>
         <v/>
       </c>
       <c r="D79" s="32" t="str">
@@ -6803,7 +6850,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R79,'New Data'!$R$16:$R$115,0),CELL("colonne",P79)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R79,'New Data'!$R$16:$R$115,0),CELL("colonne",P79)-3)),IF(OldData!P79="","",OldData!P79))</f>
         <v/>
       </c>
-      <c r="R79" s="110" t="str">
+      <c r="R79" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6814,11 +6861,11 @@
         <v/>
       </c>
       <c r="B80" s="53" t="str">
-        <f>IF(OldData!B80="","",OldData!B80)</f>
+        <f>IF(OldData!B80="","",MID(OldData!B80,2,9999))</f>
         <v/>
       </c>
       <c r="C80" s="54" t="str">
-        <f>IF(OldData!C80="","",OldData!C80)</f>
+        <f>IF(OldData!C80="","",MID(OldData!C80,2,9999))</f>
         <v/>
       </c>
       <c r="D80" s="32" t="str">
@@ -6873,7 +6920,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R80,'New Data'!$R$16:$R$115,0),CELL("colonne",P80)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R80,'New Data'!$R$16:$R$115,0),CELL("colonne",P80)-3)),IF(OldData!P80="","",OldData!P80))</f>
         <v/>
       </c>
-      <c r="R80" s="110" t="str">
+      <c r="R80" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6884,11 +6931,11 @@
         <v/>
       </c>
       <c r="B81" s="53" t="str">
-        <f>IF(OldData!B81="","",OldData!B81)</f>
+        <f>IF(OldData!B81="","",MID(OldData!B81,2,9999))</f>
         <v/>
       </c>
       <c r="C81" s="54" t="str">
-        <f>IF(OldData!C81="","",OldData!C81)</f>
+        <f>IF(OldData!C81="","",MID(OldData!C81,2,9999))</f>
         <v/>
       </c>
       <c r="D81" s="32" t="str">
@@ -6943,7 +6990,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R81,'New Data'!$R$16:$R$115,0),CELL("colonne",P81)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R81,'New Data'!$R$16:$R$115,0),CELL("colonne",P81)-3)),IF(OldData!P81="","",OldData!P81))</f>
         <v/>
       </c>
-      <c r="R81" s="110" t="str">
+      <c r="R81" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -6954,11 +7001,11 @@
         <v/>
       </c>
       <c r="B82" s="53" t="str">
-        <f>IF(OldData!B82="","",OldData!B82)</f>
+        <f>IF(OldData!B82="","",MID(OldData!B82,2,9999))</f>
         <v/>
       </c>
       <c r="C82" s="54" t="str">
-        <f>IF(OldData!C82="","",OldData!C82)</f>
+        <f>IF(OldData!C82="","",MID(OldData!C82,2,9999))</f>
         <v/>
       </c>
       <c r="D82" s="32" t="str">
@@ -7013,7 +7060,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R82,'New Data'!$R$16:$R$115,0),CELL("colonne",P82)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R82,'New Data'!$R$16:$R$115,0),CELL("colonne",P82)-3)),IF(OldData!P82="","",OldData!P82))</f>
         <v/>
       </c>
-      <c r="R82" s="110" t="str">
+      <c r="R82" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7024,11 +7071,11 @@
         <v/>
       </c>
       <c r="B83" s="53" t="str">
-        <f>IF(OldData!B83="","",OldData!B83)</f>
+        <f>IF(OldData!B83="","",MID(OldData!B83,2,9999))</f>
         <v/>
       </c>
       <c r="C83" s="54" t="str">
-        <f>IF(OldData!C83="","",OldData!C83)</f>
+        <f>IF(OldData!C83="","",MID(OldData!C83,2,9999))</f>
         <v/>
       </c>
       <c r="D83" s="32" t="str">
@@ -7083,7 +7130,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R83,'New Data'!$R$16:$R$115,0),CELL("colonne",P83)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R83,'New Data'!$R$16:$R$115,0),CELL("colonne",P83)-3)),IF(OldData!P83="","",OldData!P83))</f>
         <v/>
       </c>
-      <c r="R83" s="110" t="str">
+      <c r="R83" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7094,11 +7141,11 @@
         <v/>
       </c>
       <c r="B84" s="53" t="str">
-        <f>IF(OldData!B84="","",OldData!B84)</f>
+        <f>IF(OldData!B84="","",MID(OldData!B84,2,9999))</f>
         <v/>
       </c>
       <c r="C84" s="54" t="str">
-        <f>IF(OldData!C84="","",OldData!C84)</f>
+        <f>IF(OldData!C84="","",MID(OldData!C84,2,9999))</f>
         <v/>
       </c>
       <c r="D84" s="32" t="str">
@@ -7153,7 +7200,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R84,'New Data'!$R$16:$R$115,0),CELL("colonne",P84)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R84,'New Data'!$R$16:$R$115,0),CELL("colonne",P84)-3)),IF(OldData!P84="","",OldData!P84))</f>
         <v/>
       </c>
-      <c r="R84" s="110" t="str">
+      <c r="R84" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7164,11 +7211,11 @@
         <v/>
       </c>
       <c r="B85" s="53" t="str">
-        <f>IF(OldData!B85="","",OldData!B85)</f>
+        <f>IF(OldData!B85="","",MID(OldData!B85,2,9999))</f>
         <v/>
       </c>
       <c r="C85" s="54" t="str">
-        <f>IF(OldData!C85="","",OldData!C85)</f>
+        <f>IF(OldData!C85="","",MID(OldData!C85,2,9999))</f>
         <v/>
       </c>
       <c r="D85" s="32" t="str">
@@ -7223,7 +7270,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R85,'New Data'!$R$16:$R$115,0),CELL("colonne",P85)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R85,'New Data'!$R$16:$R$115,0),CELL("colonne",P85)-3)),IF(OldData!P85="","",OldData!P85))</f>
         <v/>
       </c>
-      <c r="R85" s="110" t="str">
+      <c r="R85" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7234,11 +7281,11 @@
         <v/>
       </c>
       <c r="B86" s="53" t="str">
-        <f>IF(OldData!B86="","",OldData!B86)</f>
+        <f>IF(OldData!B86="","",MID(OldData!B86,2,9999))</f>
         <v/>
       </c>
       <c r="C86" s="54" t="str">
-        <f>IF(OldData!C86="","",OldData!C86)</f>
+        <f>IF(OldData!C86="","",MID(OldData!C86,2,9999))</f>
         <v/>
       </c>
       <c r="D86" s="32" t="str">
@@ -7293,7 +7340,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R86,'New Data'!$R$16:$R$115,0),CELL("colonne",P86)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R86,'New Data'!$R$16:$R$115,0),CELL("colonne",P86)-3)),IF(OldData!P86="","",OldData!P86))</f>
         <v/>
       </c>
-      <c r="R86" s="110" t="str">
+      <c r="R86" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7304,11 +7351,11 @@
         <v/>
       </c>
       <c r="B87" s="53" t="str">
-        <f>IF(OldData!B87="","",OldData!B87)</f>
+        <f>IF(OldData!B87="","",MID(OldData!B87,2,9999))</f>
         <v/>
       </c>
       <c r="C87" s="54" t="str">
-        <f>IF(OldData!C87="","",OldData!C87)</f>
+        <f>IF(OldData!C87="","",MID(OldData!C87,2,9999))</f>
         <v/>
       </c>
       <c r="D87" s="32" t="str">
@@ -7363,7 +7410,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R87,'New Data'!$R$16:$R$115,0),CELL("colonne",P87)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R87,'New Data'!$R$16:$R$115,0),CELL("colonne",P87)-3)),IF(OldData!P87="","",OldData!P87))</f>
         <v/>
       </c>
-      <c r="R87" s="110" t="str">
+      <c r="R87" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7374,11 +7421,11 @@
         <v/>
       </c>
       <c r="B88" s="53" t="str">
-        <f>IF(OldData!B88="","",OldData!B88)</f>
+        <f>IF(OldData!B88="","",MID(OldData!B88,2,9999))</f>
         <v/>
       </c>
       <c r="C88" s="54" t="str">
-        <f>IF(OldData!C88="","",OldData!C88)</f>
+        <f>IF(OldData!C88="","",MID(OldData!C88,2,9999))</f>
         <v/>
       </c>
       <c r="D88" s="32" t="str">
@@ -7433,7 +7480,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R88,'New Data'!$R$16:$R$115,0),CELL("colonne",P88)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R88,'New Data'!$R$16:$R$115,0),CELL("colonne",P88)-3)),IF(OldData!P88="","",OldData!P88))</f>
         <v/>
       </c>
-      <c r="R88" s="110" t="str">
+      <c r="R88" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7444,11 +7491,11 @@
         <v/>
       </c>
       <c r="B89" s="53" t="str">
-        <f>IF(OldData!B89="","",OldData!B89)</f>
+        <f>IF(OldData!B89="","",MID(OldData!B89,2,9999))</f>
         <v/>
       </c>
       <c r="C89" s="54" t="str">
-        <f>IF(OldData!C89="","",OldData!C89)</f>
+        <f>IF(OldData!C89="","",MID(OldData!C89,2,9999))</f>
         <v/>
       </c>
       <c r="D89" s="32" t="str">
@@ -7503,7 +7550,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R89,'New Data'!$R$16:$R$115,0),CELL("colonne",P89)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R89,'New Data'!$R$16:$R$115,0),CELL("colonne",P89)-3)),IF(OldData!P89="","",OldData!P89))</f>
         <v/>
       </c>
-      <c r="R89" s="110" t="str">
+      <c r="R89" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7514,11 +7561,11 @@
         <v/>
       </c>
       <c r="B90" s="53" t="str">
-        <f>IF(OldData!B90="","",OldData!B90)</f>
+        <f>IF(OldData!B90="","",MID(OldData!B90,2,9999))</f>
         <v/>
       </c>
       <c r="C90" s="54" t="str">
-        <f>IF(OldData!C90="","",OldData!C90)</f>
+        <f>IF(OldData!C90="","",MID(OldData!C90,2,9999))</f>
         <v/>
       </c>
       <c r="D90" s="32" t="str">
@@ -7573,7 +7620,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R90,'New Data'!$R$16:$R$115,0),CELL("colonne",P90)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R90,'New Data'!$R$16:$R$115,0),CELL("colonne",P90)-3)),IF(OldData!P90="","",OldData!P90))</f>
         <v/>
       </c>
-      <c r="R90" s="110" t="str">
+      <c r="R90" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7584,11 +7631,11 @@
         <v/>
       </c>
       <c r="B91" s="53" t="str">
-        <f>IF(OldData!B91="","",OldData!B91)</f>
+        <f>IF(OldData!B91="","",MID(OldData!B91,2,9999))</f>
         <v/>
       </c>
       <c r="C91" s="54" t="str">
-        <f>IF(OldData!C91="","",OldData!C91)</f>
+        <f>IF(OldData!C91="","",MID(OldData!C91,2,9999))</f>
         <v/>
       </c>
       <c r="D91" s="32" t="str">
@@ -7643,7 +7690,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R91,'New Data'!$R$16:$R$115,0),CELL("colonne",P91)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R91,'New Data'!$R$16:$R$115,0),CELL("colonne",P91)-3)),IF(OldData!P91="","",OldData!P91))</f>
         <v/>
       </c>
-      <c r="R91" s="110" t="str">
+      <c r="R91" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7654,11 +7701,11 @@
         <v/>
       </c>
       <c r="B92" s="53" t="str">
-        <f>IF(OldData!B92="","",OldData!B92)</f>
+        <f>IF(OldData!B92="","",MID(OldData!B92,2,9999))</f>
         <v/>
       </c>
       <c r="C92" s="54" t="str">
-        <f>IF(OldData!C92="","",OldData!C92)</f>
+        <f>IF(OldData!C92="","",MID(OldData!C92,2,9999))</f>
         <v/>
       </c>
       <c r="D92" s="32" t="str">
@@ -7713,7 +7760,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R92,'New Data'!$R$16:$R$115,0),CELL("colonne",P92)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R92,'New Data'!$R$16:$R$115,0),CELL("colonne",P92)-3)),IF(OldData!P92="","",OldData!P92))</f>
         <v/>
       </c>
-      <c r="R92" s="110" t="str">
+      <c r="R92" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7724,11 +7771,11 @@
         <v/>
       </c>
       <c r="B93" s="53" t="str">
-        <f>IF(OldData!B93="","",OldData!B93)</f>
+        <f>IF(OldData!B93="","",MID(OldData!B93,2,9999))</f>
         <v/>
       </c>
       <c r="C93" s="54" t="str">
-        <f>IF(OldData!C93="","",OldData!C93)</f>
+        <f>IF(OldData!C93="","",MID(OldData!C93,2,9999))</f>
         <v/>
       </c>
       <c r="D93" s="32" t="str">
@@ -7783,7 +7830,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R93,'New Data'!$R$16:$R$115,0),CELL("colonne",P93)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R93,'New Data'!$R$16:$R$115,0),CELL("colonne",P93)-3)),IF(OldData!P93="","",OldData!P93))</f>
         <v/>
       </c>
-      <c r="R93" s="110" t="str">
+      <c r="R93" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7794,11 +7841,11 @@
         <v/>
       </c>
       <c r="B94" s="53" t="str">
-        <f>IF(OldData!B94="","",OldData!B94)</f>
+        <f>IF(OldData!B94="","",MID(OldData!B94,2,9999))</f>
         <v/>
       </c>
       <c r="C94" s="54" t="str">
-        <f>IF(OldData!C94="","",OldData!C94)</f>
+        <f>IF(OldData!C94="","",MID(OldData!C94,2,9999))</f>
         <v/>
       </c>
       <c r="D94" s="32" t="str">
@@ -7853,7 +7900,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R94,'New Data'!$R$16:$R$115,0),CELL("colonne",P94)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R94,'New Data'!$R$16:$R$115,0),CELL("colonne",P94)-3)),IF(OldData!P94="","",OldData!P94))</f>
         <v/>
       </c>
-      <c r="R94" s="110" t="str">
+      <c r="R94" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7864,11 +7911,11 @@
         <v/>
       </c>
       <c r="B95" s="53" t="str">
-        <f>IF(OldData!B95="","",OldData!B95)</f>
+        <f>IF(OldData!B95="","",MID(OldData!B95,2,9999))</f>
         <v/>
       </c>
       <c r="C95" s="54" t="str">
-        <f>IF(OldData!C95="","",OldData!C95)</f>
+        <f>IF(OldData!C95="","",MID(OldData!C95,2,9999))</f>
         <v/>
       </c>
       <c r="D95" s="32" t="str">
@@ -7923,7 +7970,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R95,'New Data'!$R$16:$R$115,0),CELL("colonne",P95)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R95,'New Data'!$R$16:$R$115,0),CELL("colonne",P95)-3)),IF(OldData!P95="","",OldData!P95))</f>
         <v/>
       </c>
-      <c r="R95" s="110" t="str">
+      <c r="R95" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7934,11 +7981,11 @@
         <v/>
       </c>
       <c r="B96" s="53" t="str">
-        <f>IF(OldData!B96="","",OldData!B96)</f>
+        <f>IF(OldData!B96="","",MID(OldData!B96,2,9999))</f>
         <v/>
       </c>
       <c r="C96" s="54" t="str">
-        <f>IF(OldData!C96="","",OldData!C96)</f>
+        <f>IF(OldData!C96="","",MID(OldData!C96,2,9999))</f>
         <v/>
       </c>
       <c r="D96" s="32" t="str">
@@ -7993,7 +8040,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R96,'New Data'!$R$16:$R$115,0),CELL("colonne",P96)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R96,'New Data'!$R$16:$R$115,0),CELL("colonne",P96)-3)),IF(OldData!P96="","",OldData!P96))</f>
         <v/>
       </c>
-      <c r="R96" s="110" t="str">
+      <c r="R96" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8004,11 +8051,11 @@
         <v/>
       </c>
       <c r="B97" s="53" t="str">
-        <f>IF(OldData!B97="","",OldData!B97)</f>
+        <f>IF(OldData!B97="","",MID(OldData!B97,2,9999))</f>
         <v/>
       </c>
       <c r="C97" s="54" t="str">
-        <f>IF(OldData!C97="","",OldData!C97)</f>
+        <f>IF(OldData!C97="","",MID(OldData!C97,2,9999))</f>
         <v/>
       </c>
       <c r="D97" s="32" t="str">
@@ -8063,7 +8110,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R97,'New Data'!$R$16:$R$115,0),CELL("colonne",P97)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R97,'New Data'!$R$16:$R$115,0),CELL("colonne",P97)-3)),IF(OldData!P97="","",OldData!P97))</f>
         <v/>
       </c>
-      <c r="R97" s="110" t="str">
+      <c r="R97" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8074,11 +8121,11 @@
         <v/>
       </c>
       <c r="B98" s="53" t="str">
-        <f>IF(OldData!B98="","",OldData!B98)</f>
+        <f>IF(OldData!B98="","",MID(OldData!B98,2,9999))</f>
         <v/>
       </c>
       <c r="C98" s="54" t="str">
-        <f>IF(OldData!C98="","",OldData!C98)</f>
+        <f>IF(OldData!C98="","",MID(OldData!C98,2,9999))</f>
         <v/>
       </c>
       <c r="D98" s="32" t="str">
@@ -8133,7 +8180,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R98,'New Data'!$R$16:$R$115,0),CELL("colonne",P98)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R98,'New Data'!$R$16:$R$115,0),CELL("colonne",P98)-3)),IF(OldData!P98="","",OldData!P98))</f>
         <v/>
       </c>
-      <c r="R98" s="110" t="str">
+      <c r="R98" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8144,11 +8191,11 @@
         <v/>
       </c>
       <c r="B99" s="53" t="str">
-        <f>IF(OldData!B99="","",OldData!B99)</f>
+        <f>IF(OldData!B99="","",MID(OldData!B99,2,9999))</f>
         <v/>
       </c>
       <c r="C99" s="54" t="str">
-        <f>IF(OldData!C99="","",OldData!C99)</f>
+        <f>IF(OldData!C99="","",MID(OldData!C99,2,9999))</f>
         <v/>
       </c>
       <c r="D99" s="32" t="str">
@@ -8203,7 +8250,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R99,'New Data'!$R$16:$R$115,0),CELL("colonne",P99)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R99,'New Data'!$R$16:$R$115,0),CELL("colonne",P99)-3)),IF(OldData!P99="","",OldData!P99))</f>
         <v/>
       </c>
-      <c r="R99" s="110" t="str">
+      <c r="R99" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8214,11 +8261,11 @@
         <v/>
       </c>
       <c r="B100" s="53" t="str">
-        <f>IF(OldData!B100="","",OldData!B100)</f>
+        <f>IF(OldData!B100="","",MID(OldData!B100,2,9999))</f>
         <v/>
       </c>
       <c r="C100" s="54" t="str">
-        <f>IF(OldData!C100="","",OldData!C100)</f>
+        <f>IF(OldData!C100="","",MID(OldData!C100,2,9999))</f>
         <v/>
       </c>
       <c r="D100" s="32" t="str">
@@ -8273,7 +8320,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R100,'New Data'!$R$16:$R$115,0),CELL("colonne",P100)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R100,'New Data'!$R$16:$R$115,0),CELL("colonne",P100)-3)),IF(OldData!P100="","",OldData!P100))</f>
         <v/>
       </c>
-      <c r="R100" s="110" t="str">
+      <c r="R100" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8284,11 +8331,11 @@
         <v/>
       </c>
       <c r="B101" s="53" t="str">
-        <f>IF(OldData!B101="","",OldData!B101)</f>
+        <f>IF(OldData!B101="","",MID(OldData!B101,2,9999))</f>
         <v/>
       </c>
       <c r="C101" s="54" t="str">
-        <f>IF(OldData!C101="","",OldData!C101)</f>
+        <f>IF(OldData!C101="","",MID(OldData!C101,2,9999))</f>
         <v/>
       </c>
       <c r="D101" s="32" t="str">
@@ -8343,7 +8390,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R101,'New Data'!$R$16:$R$115,0),CELL("colonne",P101)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R101,'New Data'!$R$16:$R$115,0),CELL("colonne",P101)-3)),IF(OldData!P101="","",OldData!P101))</f>
         <v/>
       </c>
-      <c r="R101" s="110" t="str">
+      <c r="R101" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8354,11 +8401,11 @@
         <v/>
       </c>
       <c r="B102" s="53" t="str">
-        <f>IF(OldData!B102="","",OldData!B102)</f>
+        <f>IF(OldData!B102="","",MID(OldData!B102,2,9999))</f>
         <v/>
       </c>
       <c r="C102" s="54" t="str">
-        <f>IF(OldData!C102="","",OldData!C102)</f>
+        <f>IF(OldData!C102="","",MID(OldData!C102,2,9999))</f>
         <v/>
       </c>
       <c r="D102" s="32" t="str">
@@ -8413,7 +8460,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R102,'New Data'!$R$16:$R$115,0),CELL("colonne",P102)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R102,'New Data'!$R$16:$R$115,0),CELL("colonne",P102)-3)),IF(OldData!P102="","",OldData!P102))</f>
         <v/>
       </c>
-      <c r="R102" s="110" t="str">
+      <c r="R102" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8424,11 +8471,11 @@
         <v/>
       </c>
       <c r="B103" s="53" t="str">
-        <f>IF(OldData!B103="","",OldData!B103)</f>
+        <f>IF(OldData!B103="","",MID(OldData!B103,2,9999))</f>
         <v/>
       </c>
       <c r="C103" s="54" t="str">
-        <f>IF(OldData!C103="","",OldData!C103)</f>
+        <f>IF(OldData!C103="","",MID(OldData!C103,2,9999))</f>
         <v/>
       </c>
       <c r="D103" s="32" t="str">
@@ -8483,7 +8530,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R103,'New Data'!$R$16:$R$115,0),CELL("colonne",P103)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R103,'New Data'!$R$16:$R$115,0),CELL("colonne",P103)-3)),IF(OldData!P103="","",OldData!P103))</f>
         <v/>
       </c>
-      <c r="R103" s="110" t="str">
+      <c r="R103" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8494,11 +8541,11 @@
         <v/>
       </c>
       <c r="B104" s="53" t="str">
-        <f>IF(OldData!B104="","",OldData!B104)</f>
+        <f>IF(OldData!B104="","",MID(OldData!B104,2,9999))</f>
         <v/>
       </c>
       <c r="C104" s="54" t="str">
-        <f>IF(OldData!C104="","",OldData!C104)</f>
+        <f>IF(OldData!C104="","",MID(OldData!C104,2,9999))</f>
         <v/>
       </c>
       <c r="D104" s="32" t="str">
@@ -8553,7 +8600,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R104,'New Data'!$R$16:$R$115,0),CELL("colonne",P104)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R104,'New Data'!$R$16:$R$115,0),CELL("colonne",P104)-3)),IF(OldData!P104="","",OldData!P104))</f>
         <v/>
       </c>
-      <c r="R104" s="110" t="str">
+      <c r="R104" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8564,11 +8611,11 @@
         <v/>
       </c>
       <c r="B105" s="53" t="str">
-        <f>IF(OldData!B105="","",OldData!B105)</f>
+        <f>IF(OldData!B105="","",MID(OldData!B105,2,9999))</f>
         <v/>
       </c>
       <c r="C105" s="54" t="str">
-        <f>IF(OldData!C105="","",OldData!C105)</f>
+        <f>IF(OldData!C105="","",MID(OldData!C105,2,9999))</f>
         <v/>
       </c>
       <c r="D105" s="32" t="str">
@@ -8623,7 +8670,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R105,'New Data'!$R$16:$R$115,0),CELL("colonne",P105)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R105,'New Data'!$R$16:$R$115,0),CELL("colonne",P105)-3)),IF(OldData!P105="","",OldData!P105))</f>
         <v/>
       </c>
-      <c r="R105" s="110" t="str">
+      <c r="R105" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8634,11 +8681,11 @@
         <v/>
       </c>
       <c r="B106" s="53" t="str">
-        <f>IF(OldData!B106="","",OldData!B106)</f>
+        <f>IF(OldData!B106="","",MID(OldData!B106,2,9999))</f>
         <v/>
       </c>
       <c r="C106" s="54" t="str">
-        <f>IF(OldData!C106="","",OldData!C106)</f>
+        <f>IF(OldData!C106="","",MID(OldData!C106,2,9999))</f>
         <v/>
       </c>
       <c r="D106" s="32" t="str">
@@ -8693,7 +8740,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R106,'New Data'!$R$16:$R$115,0),CELL("colonne",P106)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R106,'New Data'!$R$16:$R$115,0),CELL("colonne",P106)-3)),IF(OldData!P106="","",OldData!P106))</f>
         <v/>
       </c>
-      <c r="R106" s="110" t="str">
+      <c r="R106" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8704,11 +8751,11 @@
         <v/>
       </c>
       <c r="B107" s="53" t="str">
-        <f>IF(OldData!B107="","",OldData!B107)</f>
+        <f>IF(OldData!B107="","",MID(OldData!B107,2,9999))</f>
         <v/>
       </c>
       <c r="C107" s="54" t="str">
-        <f>IF(OldData!C107="","",OldData!C107)</f>
+        <f>IF(OldData!C107="","",MID(OldData!C107,2,9999))</f>
         <v/>
       </c>
       <c r="D107" s="32" t="str">
@@ -8763,7 +8810,7 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R107,'New Data'!$R$16:$R$115,0),CELL("colonne",P107)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R107,'New Data'!$R$16:$R$115,0),CELL("colonne",P107)-3)),IF(OldData!P107="","",OldData!P107))</f>
         <v/>
       </c>
-      <c r="R107" s="110" t="str">
+      <c r="R107" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8774,11 +8821,11 @@
         <v/>
       </c>
       <c r="B108" s="53" t="str">
-        <f>IF(OldData!B108="","",OldData!B108)</f>
+        <f>IF(OldData!B108="","",MID(OldData!B108,2,9999))</f>
         <v/>
       </c>
       <c r="C108" s="54" t="str">
-        <f>IF(OldData!C108="","",OldData!C108)</f>
+        <f>IF(OldData!C108="","",MID(OldData!C108,2,9999))</f>
         <v/>
       </c>
       <c r="D108" s="32" t="str">
@@ -8834,7 +8881,7 @@
         <v/>
       </c>
       <c r="Q108" s="44"/>
-      <c r="R108" s="110" t="str">
+      <c r="R108" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8845,11 +8892,11 @@
         <v/>
       </c>
       <c r="B109" s="53" t="str">
-        <f>IF(OldData!B109="","",OldData!B109)</f>
+        <f>IF(OldData!B109="","",MID(OldData!B109,2,9999))</f>
         <v/>
       </c>
       <c r="C109" s="54" t="str">
-        <f>IF(OldData!C109="","",OldData!C109)</f>
+        <f>IF(OldData!C109="","",MID(OldData!C109,2,9999))</f>
         <v/>
       </c>
       <c r="D109" s="32" t="str">
@@ -8905,7 +8952,7 @@
         <v/>
       </c>
       <c r="Q109" s="44"/>
-      <c r="R109" s="110" t="str">
+      <c r="R109" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8916,11 +8963,11 @@
         <v/>
       </c>
       <c r="B110" s="53" t="str">
-        <f>IF(OldData!B110="","",OldData!B110)</f>
+        <f>IF(OldData!B110="","",MID(OldData!B110,2,9999))</f>
         <v/>
       </c>
       <c r="C110" s="54" t="str">
-        <f>IF(OldData!C110="","",OldData!C110)</f>
+        <f>IF(OldData!C110="","",MID(OldData!C110,2,9999))</f>
         <v/>
       </c>
       <c r="D110" s="32" t="str">
@@ -8976,7 +9023,7 @@
         <v/>
       </c>
       <c r="Q110" s="44"/>
-      <c r="R110" s="110" t="str">
+      <c r="R110" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -8987,11 +9034,11 @@
         <v/>
       </c>
       <c r="B111" s="53" t="str">
-        <f>IF(OldData!B111="","",OldData!B111)</f>
+        <f>IF(OldData!B111="","",MID(OldData!B111,2,9999))</f>
         <v/>
       </c>
       <c r="C111" s="54" t="str">
-        <f>IF(OldData!C111="","",OldData!C111)</f>
+        <f>IF(OldData!C111="","",MID(OldData!C111,2,9999))</f>
         <v/>
       </c>
       <c r="D111" s="32" t="str">
@@ -9047,7 +9094,7 @@
         <v/>
       </c>
       <c r="Q111" s="44"/>
-      <c r="R111" s="110" t="str">
+      <c r="R111" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -9058,11 +9105,11 @@
         <v/>
       </c>
       <c r="B112" s="53" t="str">
-        <f>IF(OldData!B112="","",OldData!B112)</f>
+        <f>IF(OldData!B112="","",MID(OldData!B112,2,9999))</f>
         <v/>
       </c>
       <c r="C112" s="54" t="str">
-        <f>IF(OldData!C112="","",OldData!C112)</f>
+        <f>IF(OldData!C112="","",MID(OldData!C112,2,9999))</f>
         <v/>
       </c>
       <c r="D112" s="32" t="str">
@@ -9118,7 +9165,7 @@
         <v/>
       </c>
       <c r="Q112" s="44"/>
-      <c r="R112" s="110" t="str">
+      <c r="R112" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -9129,11 +9176,11 @@
         <v/>
       </c>
       <c r="B113" s="53" t="str">
-        <f>IF(OldData!B113="","",OldData!B113)</f>
+        <f>IF(OldData!B113="","",MID(OldData!B113,2,9999))</f>
         <v/>
       </c>
       <c r="C113" s="54" t="str">
-        <f>IF(OldData!C113="","",OldData!C113)</f>
+        <f>IF(OldData!C113="","",MID(OldData!C113,2,9999))</f>
         <v/>
       </c>
       <c r="D113" s="32" t="str">
@@ -9189,22 +9236,22 @@
         <v/>
       </c>
       <c r="Q113" s="44"/>
-      <c r="R113" s="110" t="str">
+      <c r="R113" s="109" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="43" t="str">
         <f>IF(OldData!A114="","",OldData!A114)</f>
         <v/>
       </c>
       <c r="B114" s="60" t="str">
-        <f>IF(OldData!B114="","",OldData!B114)</f>
+        <f>IF(OldData!B114="","",MID(OldData!B114,2,9999))</f>
         <v/>
       </c>
       <c r="C114" s="61" t="str">
-        <f>IF(OldData!C114="","",OldData!C114)</f>
+        <f>IF(OldData!C114="","",MID(OldData!C114,2,9999))</f>
         <v/>
       </c>
       <c r="D114" s="80" t="str">
@@ -9259,12 +9306,12 @@
         <f ca="1">IFERROR(IF(INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R114,'New Data'!$R$16:$R$115,0),CELL("colonne",P114)-3)="","",INDEX('New Data'!$D$16:$N$115,MATCH('INSPECTION QUALITE DIM INSTRUM'!$R114,'New Data'!$R$16:$R$115,0),CELL("colonne",P114)-3)),IF(OldData!P114="","",OldData!P114))</f>
         <v/>
       </c>
-      <c r="R114" s="110" t="str">
+      <c r="R114" s="109" t="str">
         <f t="shared" ref="R114" si="3">B114&amp;C114</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" spans="1:18" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
@@ -9313,6 +9360,7 @@
     <oddFooter>&amp;RPage &amp;P de &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9376,64 +9424,64 @@
       <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="121" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="120" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="120" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="120" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="121"/>
+      <c r="B9" s="120"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="H10" s="113"/>
-      <c r="I10" s="114" t="s">
+      <c r="H10" s="112"/>
+      <c r="I10" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="114"/>
-      <c r="K10" s="114"/>
-      <c r="L10" s="115"/>
-      <c r="N10" s="111"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="114"/>
+      <c r="N10" s="110"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="H11" s="116">
+      <c r="H11" s="115">
         <v>1</v>
       </c>
-      <c r="I11" s="111" t="s">
+      <c r="I11" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
-      <c r="L11" s="117"/>
-      <c r="N11" s="111"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="110"/>
+      <c r="L11" s="116"/>
+      <c r="N11" s="110"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="H12" s="118">
+      <c r="H12" s="117">
         <v>2</v>
       </c>
-      <c r="I12" s="119" t="s">
+      <c r="I12" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="120"/>
-      <c r="N12" s="111"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="119"/>
+      <c r="N12" s="110"/>
     </row>
     <row r="13" spans="1:20" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="112"/>
+      <c r="H13" s="111"/>
     </row>
     <row r="14" spans="1:20" s="44" customFormat="1" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="86"/>
@@ -12187,10 +12235,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="81"/>
+  </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>